<commit_message>
learned how to insert empty rows and cols
</commit_message>
<xml_diff>
--- a/sample_insert_columns.xlsx
+++ b/sample_insert_columns.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,12 +427,12 @@
           <t>ID</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Math</t>
         </is>
@@ -442,10 +442,10 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="G2" t="n">
         <v>79</v>
       </c>
-      <c r="D2" t="n">
+      <c r="H2" t="n">
         <v>54</v>
       </c>
     </row>
@@ -453,10 +453,10 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="G3" t="n">
         <v>68</v>
       </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
         <v>75</v>
       </c>
     </row>
@@ -464,10 +464,10 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="n">
+      <c r="G4" t="n">
         <v>42</v>
       </c>
-      <c r="D4" t="n">
+      <c r="H4" t="n">
         <v>21</v>
       </c>
     </row>
@@ -475,10 +475,10 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
+      <c r="G5" t="n">
         <v>78</v>
       </c>
-      <c r="D5" t="n">
+      <c r="H5" t="n">
         <v>83</v>
       </c>
     </row>
@@ -486,10 +486,10 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="n">
+      <c r="G6" t="n">
         <v>59</v>
       </c>
-      <c r="D6" t="n">
+      <c r="H6" t="n">
         <v>24</v>
       </c>
     </row>
@@ -497,10 +497,10 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="n">
+      <c r="G7" t="n">
         <v>41</v>
       </c>
-      <c r="D7" t="n">
+      <c r="H7" t="n">
         <v>42</v>
       </c>
     </row>
@@ -508,10 +508,10 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="n">
+      <c r="G8" t="n">
         <v>78</v>
       </c>
-      <c r="D8" t="n">
+      <c r="H8" t="n">
         <v>59</v>
       </c>
     </row>
@@ -519,10 +519,10 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="C9" t="n">
+      <c r="G9" t="n">
         <v>55</v>
       </c>
-      <c r="D9" t="n">
+      <c r="H9" t="n">
         <v>70</v>
       </c>
     </row>
@@ -530,10 +530,10 @@
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="C10" t="n">
+      <c r="G10" t="n">
         <v>99</v>
       </c>
-      <c r="D10" t="n">
+      <c r="H10" t="n">
         <v>37</v>
       </c>
     </row>
@@ -541,10 +541,10 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="C11" t="n">
+      <c r="G11" t="n">
         <v>65</v>
       </c>
-      <c r="D11" t="n">
+      <c r="H11" t="n">
         <v>13</v>
       </c>
     </row>

</xml_diff>